<commit_message>
Improvements to config and user data folders
</commit_message>
<xml_diff>
--- a/CI/TestSQL/02.TestData/Group+Attribute/CreateGroup.xlsx
+++ b/CI/TestSQL/02.TestData/Group+Attribute/CreateGroup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahHenney\Documents\GitSources\crds-angular\CI\TestSQL\02.TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SarahHenney\Documents\GitSources\crds-angular\CI\TestSQL\02.TestData\Group+Attribute\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
   <si>
     <t>Target_Size</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>R_Child_Care_Available</t>
+  </si>
+  <si>
+    <t>Meeting_Day</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>Available_Online</t>
   </si>
 </sst>
 </file>
@@ -649,10 +658,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1008,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P19"/>
+  <dimension ref="A1:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1026,15 +1036,17 @@
     <col min="8" max="8" width="24.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.53125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.53125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.9296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1328125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.53125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.53125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.9296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1066,25 +1078,31 @@
         <v>41</v>
       </c>
       <c r="K1" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
         <v>33</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>35</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1109,20 +1127,20 @@
       <c r="H2" t="s">
         <v>4</v>
       </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -1147,20 +1165,20 @@
       <c r="H3" t="s">
         <v>4</v>
       </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
         <v>39</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>40</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1183,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1209,7 +1227,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1234,14 +1252,14 @@
       <c r="I6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <v>4</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1263,14 +1281,14 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>10</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -1295,23 +1313,23 @@
       <c r="H8" t="s">
         <v>4</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
         <v>58</v>
       </c>
-      <c r="N8" t="s">
+      <c r="P8" t="s">
         <v>39</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>40</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -1336,23 +1354,23 @@
       <c r="H9" t="s">
         <v>4</v>
       </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-      <c r="M9">
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>58</v>
       </c>
-      <c r="N9" t="s">
+      <c r="P9" t="s">
         <v>39</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1375,7 +1393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -1398,7 +1416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1423,20 +1441,20 @@
       <c r="H12" t="s">
         <v>4</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="N12" t="s">
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
         <v>39</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>40</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -1458,11 +1476,11 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1484,11 +1502,11 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1510,11 +1528,11 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1542,11 +1560,11 @@
       <c r="J16">
         <v>1</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -1574,14 +1592,20 @@
       <c r="J17">
         <v>1</v>
       </c>
-      <c r="K17" s="2">
+      <c r="K17" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="2">
         <v>0.70833333333333337</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="3">
+        <v>1</v>
+      </c>
+      <c r="O17">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -1609,11 +1633,11 @@
       <c r="J18">
         <v>1</v>
       </c>
-      <c r="M18">
+      <c r="O18">
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>31</v>
       </c>
@@ -1641,11 +1665,12 @@
       <c r="J19">
         <v>1</v>
       </c>
-      <c r="M19">
+      <c r="O19">
         <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>